<commit_message>
Before preparing for DATE
</commit_message>
<xml_diff>
--- a/for_paper_icces/experiments/summary.xlsx
+++ b/for_paper_icces/experiments/summary.xlsx
@@ -225,6 +225,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -293,7 +294,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -305,7 +306,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -333,7 +334,7 @@
   <dimension ref="A1:F40"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I23" activeCellId="0" sqref="I23"/>
+      <selection pane="topLeft" activeCell="C40" activeCellId="0" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -938,7 +939,7 @@
         <v>10</v>
       </c>
       <c r="C39" s="1" t="n">
-        <v>1.40000000000001</v>
+        <v>1.2</v>
       </c>
       <c r="D39" s="1" t="n">
         <v>1.36</v>
@@ -956,7 +957,7 @@
         <v>11</v>
       </c>
       <c r="C40" s="1" t="n">
-        <v>1.94</v>
+        <v>1.34</v>
       </c>
       <c r="D40" s="1" t="n">
         <v>1.54</v>
@@ -1010,7 +1011,7 @@
   <dimension ref="A1:K40"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H4" activeCellId="0" sqref="H4"/>
+      <selection pane="topLeft" activeCell="C40" activeCellId="0" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1759,7 +1760,7 @@
         <v>10</v>
       </c>
       <c r="C39" s="1" t="n">
-        <v>1.40000000000001</v>
+        <v>1.2</v>
       </c>
       <c r="D39" s="1" t="n">
         <v>1.36</v>
@@ -1777,7 +1778,7 @@
         <v>11</v>
       </c>
       <c r="C40" s="1" t="n">
-        <v>1.94</v>
+        <v>1.34</v>
       </c>
       <c r="D40" s="1" t="n">
         <v>1.54</v>
@@ -1815,7 +1816,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -1831,7 +1832,7 @@
   <dimension ref="A1:F38"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D24" activeCellId="0" sqref="D24"/>
+      <selection pane="topLeft" activeCell="D28" activeCellId="0" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2224,11 +2225,11 @@
         <v>51.41</v>
       </c>
       <c r="D28" s="0" t="n">
-        <v>52.81</v>
+        <v>52.61</v>
       </c>
       <c r="F28" s="0" t="n">
         <f aca="false">D28-C28</f>
-        <v>1.40000000000001</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2239,11 +2240,11 @@
         <v>51.53</v>
       </c>
       <c r="D29" s="0" t="n">
-        <v>53.47</v>
+        <v>52.87</v>
       </c>
       <c r="F29" s="0" t="n">
         <f aca="false">D29-C29</f>
-        <v>1.94</v>
+        <v>1.34</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2384,7 +2385,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>